<commit_message>
modification of base tree in terms of test inputs
</commit_message>
<xml_diff>
--- a/data/test_inputs/preprocessing/performance_format/Performance_90_PP_Sup.xlsx
+++ b/data/test_inputs/preprocessing/performance_format/Performance_90_PP_Sup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/performance_format/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/test_inputs/preprocessing/performance_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF694C16-3C43-7040-8E22-C7057F5235E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F852992-F851-6D41-80AF-70D951D4E521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8080" yWindow="500" windowWidth="21260" windowHeight="17400" activeTab="1" xr2:uid="{968F1003-936B-E54A-97BA-F1A20154874A}"/>
+    <workbookView xWindow="8080" yWindow="500" windowWidth="21260" windowHeight="17400" xr2:uid="{968F1003-936B-E54A-97BA-F1A20154874A}"/>
   </bookViews>
   <sheets>
     <sheet name="performance_params_90" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,6 @@
     <t>Alternative_Param</t>
   </si>
   <si>
-    <t>e_modulus</t>
-  </si>
-  <si>
-    <t>tensile_strain_at_break</t>
-  </si>
-  <si>
-    <t>tensile_yield_strength</t>
-  </si>
-  <si>
     <t>PP_Sup_virgin</t>
   </si>
   <si>
@@ -56,6 +47,15 @@
   </si>
   <si>
     <t>Inversion</t>
+  </si>
+  <si>
+    <t>e_modulus_90</t>
+  </si>
+  <si>
+    <t>tensile_strain_at_break_90</t>
+  </si>
+  <si>
+    <t>tensile_yield_strength_90</t>
   </si>
 </sst>
 </file>
@@ -119,12 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -450,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D55A5A-B7EB-8045-ACFE-203E25D14010}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -466,61 +465,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>6</v>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
         <v>743</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>756</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>756</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
         <v>20</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>15</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>15</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
         <v>16</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>15</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>15</v>
       </c>
       <c r="E4" s="1"/>
@@ -540,65 +539,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0EF1CD5-9F5E-A145-8E77-4736678974EB}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>900</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7">
+      <c r="B4" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="7">
-        <v>900</v>
-      </c>
-      <c r="D2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="7">
-        <v>25</v>
-      </c>
-      <c r="D3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>16</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="6">
         <v>1</v>
       </c>
     </row>

</xml_diff>